<commit_message>
cap nhat bang diem
</commit_message>
<xml_diff>
--- a/DSSV/ds_20161.xlsx
+++ b/DSSV/ds_20161.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20400" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="177">
   <si>
     <t>AB</t>
   </si>
@@ -498,27 +498,15 @@
     <t>Đến hết tuần 18 (dự phòng, ôn tập)</t>
   </si>
   <si>
-    <t>tuần 15: nhắc nộp báo cáo.</t>
-  </si>
-  <si>
     <t>Trình bầy+chương trình+báo cáo</t>
   </si>
   <si>
     <t>(+) bắt buộc phải có nội dung làm rõ các câu hỏi sau: thu thập như thế nào? hệ thống hỗ trợ các kiểu truy vấn gì? Thực hiện truy vấn ntn?</t>
   </si>
   <si>
-    <t>(+) demo hoạt động của hệ thống.</t>
-  </si>
-  <si>
     <t>(+) vận hành hệ thống ntn? Kế hoạch triển khai?</t>
   </si>
   <si>
-    <t>*hệ thông nói là hoàn chỉnh: có tính cập nhật dữ liệu chỉ mục v.v.</t>
-  </si>
-  <si>
-    <t>Thời gian cho mỗi nhóm 15', các thành viên có mặt là bắt buộc.</t>
-  </si>
-  <si>
     <t>Báo cáo: tuần 16 -&gt; Lên lịch -&gt; các nhóm bảo vệ theo đúng trình tự</t>
   </si>
   <si>
@@ -537,28 +525,28 @@
     <t>demo</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>prj</t>
   </si>
   <si>
-    <t>7.5</t>
-  </si>
-  <si>
-    <t>8.0</t>
-  </si>
-  <si>
-    <t>9.0</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>8.0(7.5+)</t>
+    <t>8,0(7,5+)</t>
+  </si>
+  <si>
+    <t>tuần 15: nhắc nộp báo cáo,</t>
+  </si>
+  <si>
+    <t>(+) demo hoạt động của hệ thống,</t>
+  </si>
+  <si>
+    <t>*hệ thông nói là hoàn chỉnh: có tính cập nhật dữ liệu chỉ mục v,v,</t>
+  </si>
+  <si>
+    <t>Thời gian cho mỗi nhóm 15', các thành viên có mặt là bắt buộc,</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>bonus</t>
   </si>
 </sst>
 </file>
@@ -572,7 +560,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -580,7 +568,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -916,17 +904,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="24.625" customWidth="1"/>
-    <col min="9" max="9" width="20.375" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +1431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +1619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1760,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1819,7 +1807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +1901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +1995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -2054,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -2148,7 +2136,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2230,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -2383,7 +2371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2430,7 +2418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2618,7 +2606,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -2712,7 +2700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +2747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -2853,7 +2841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +2888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -2994,7 +2982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -3041,7 +3029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +3076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -3135,7 +3123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -3182,7 +3170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
@@ -3229,7 +3217,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -3276,7 +3264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +3311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -3370,7 +3358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -3417,7 +3405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3464,7 +3452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3518,27 +3506,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="5.125" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>176</v>
+      </c>
       <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3551,14 +3545,18 @@
       <c r="D2" t="s">
         <v>133</v>
       </c>
-      <c r="F2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f>F2+G2</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3571,14 +3569,18 @@
       <c r="D3" t="s">
         <v>134</v>
       </c>
-      <c r="F3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>7.5</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H78" si="0">F3+G3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3591,344 +3593,410 @@
       <c r="D4" t="s">
         <v>136</v>
       </c>
-      <c r="F4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>7.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>7.5</v>
+      </c>
+      <c r="H5">
+        <f>F5+G5</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
         <v>138</v>
       </c>
-      <c r="G5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="G6">
+        <v>8.5</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>140</v>
       </c>
-      <c r="G6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8">
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <f>F8+G8</f>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s">
         <v>142</v>
       </c>
-      <c r="G7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="G9">
+        <v>7.5</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10">
+        <v>7.5</v>
+      </c>
+      <c r="H10">
+        <f>F10+G10</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="s">
+        <v>170</v>
+      </c>
+      <c r="H11" t="e">
+        <f>F11+G11</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
         <v>145</v>
       </c>
-      <c r="F8" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" t="s">
         <v>147</v>
       </c>
-      <c r="F9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13">
+        <v>8.5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14">
+        <v>8.5</v>
+      </c>
+      <c r="H14">
+        <f>F14+G14</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
         <v>136</v>
       </c>
-      <c r="F10" t="s">
-        <v>173</v>
-      </c>
-      <c r="G10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15">
+        <v>7.5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F11" t="s">
-        <v>173</v>
-      </c>
-      <c r="G11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="F16">
+        <v>0.5</v>
+      </c>
+      <c r="G16">
+        <v>8.5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
         <v>136</v>
       </c>
-      <c r="F12" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="F17">
+        <v>0.5</v>
+      </c>
+      <c r="G17">
+        <v>7.5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18">
+        <v>0.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>170</v>
+      </c>
+      <c r="H18" t="e">
+        <f>F18+G18</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
         <v>138</v>
       </c>
-      <c r="F13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="F19">
+        <v>0.5</v>
+      </c>
+      <c r="G19">
+        <v>8.5</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <f>F20+G20</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
         <v>138</v>
       </c>
-      <c r="F14" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>8.5</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F15" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>25</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D16" t="s">
-        <v>140</v>
-      </c>
-      <c r="G16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>27</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" t="s">
-        <v>147</v>
-      </c>
-      <c r="F18" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>33</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F20" t="s">
-        <v>173</v>
-      </c>
-      <c r="G20" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>34</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" t="s">
-        <v>142</v>
-      </c>
-      <c r="G21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>130</v>
@@ -3936,588 +4004,726 @@
       <c r="D22" t="s">
         <v>145</v>
       </c>
-      <c r="F22" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>0.5</v>
+      </c>
+      <c r="G22">
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
-      </c>
-      <c r="F23" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="F23">
+        <v>0.5</v>
+      </c>
+      <c r="G23">
+        <v>8.5</v>
+      </c>
+      <c r="H23">
+        <f>F23+G23</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" t="s">
-        <v>148</v>
-      </c>
-      <c r="F24" t="s">
-        <v>173</v>
+        <v>131</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
       </c>
       <c r="G24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="H24" t="e">
+        <f>F24+G24</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" t="s">
-        <v>146</v>
-      </c>
-      <c r="F25" t="s">
-        <v>174</v>
+        <v>131</v>
+      </c>
+      <c r="E25" t="s">
+        <v>151</v>
       </c>
       <c r="G25" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="H25" t="e">
+        <f>F25+G25</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26">
+        <v>8</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" t="s">
+        <v>170</v>
+      </c>
+      <c r="H27" t="e">
+        <f>F27+G27</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
         <v>132</v>
       </c>
-      <c r="F26" t="s">
-        <v>174</v>
-      </c>
-      <c r="G26" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>45</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" t="s">
-        <v>173</v>
-      </c>
-      <c r="G27" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>47</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" t="s">
-        <v>134</v>
-      </c>
-      <c r="G28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D29" t="s">
-        <v>150</v>
-      </c>
-      <c r="F29" t="s">
-        <v>173</v>
-      </c>
-      <c r="G29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+      <c r="G29">
+        <v>8.5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D30" t="s">
-        <v>142</v>
-      </c>
-      <c r="F30" t="s">
-        <v>173</v>
+        <v>131</v>
+      </c>
+      <c r="E30" t="s">
+        <v>151</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="H30" t="e">
+        <f>F30+G30</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <f>F31+G31</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+      <c r="G32">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D33" t="s">
-        <v>136</v>
-      </c>
-      <c r="F33" t="s">
-        <v>173</v>
-      </c>
-      <c r="G33" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="G33">
+        <v>7.5</v>
+      </c>
+      <c r="H33">
+        <f>F33+G33</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="F34">
+        <v>0.5</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="G35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>7.5</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36">
+        <v>0.5</v>
+      </c>
+      <c r="G36">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
-      </c>
-      <c r="G37" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="F37">
+        <v>0.5</v>
+      </c>
+      <c r="G37">
+        <v>7.5</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E38" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" t="s">
-        <v>173</v>
-      </c>
-      <c r="G38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D38" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+      <c r="G38">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="G39">
+        <v>9</v>
+      </c>
+      <c r="H39">
+        <f>F39+G39</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D40" t="s">
-        <v>139</v>
-      </c>
-      <c r="F40" t="s">
-        <v>173</v>
-      </c>
-      <c r="G40" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>9</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E41" t="s">
-        <v>151</v>
-      </c>
-      <c r="G41" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41">
+        <v>8.5</v>
+      </c>
+      <c r="H41">
+        <f>F41+G41</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E43" t="s">
-        <v>151</v>
-      </c>
-      <c r="G43" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43">
+        <v>0.5</v>
+      </c>
+      <c r="G43">
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <f>F43+G43</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E44" t="s">
-        <v>151</v>
-      </c>
-      <c r="G44" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44">
+        <v>8.5</v>
+      </c>
+      <c r="H44">
+        <f>F44+G44</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D45" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" t="s">
-        <v>173</v>
-      </c>
-      <c r="G45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>152</v>
+      </c>
+      <c r="H45">
+        <f>F45+G45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D46" t="s">
-        <v>137</v>
-      </c>
-      <c r="G46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="F46">
+        <v>0.5</v>
+      </c>
+      <c r="G46">
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D47" t="s">
-        <v>148</v>
-      </c>
-      <c r="G47" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>152</v>
+      </c>
+      <c r="H47">
+        <f>F47+G47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
-      </c>
-      <c r="G48" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="G48">
+        <v>7.5</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" t="s">
-        <v>173</v>
-      </c>
-      <c r="G49" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="F49">
+        <v>0.5</v>
+      </c>
+      <c r="G49">
+        <v>9</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D50" t="s">
-        <v>138</v>
-      </c>
-      <c r="G50" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>152</v>
+      </c>
+      <c r="H50">
+        <f>F50+G50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D51" t="s">
+        <v>142</v>
+      </c>
+      <c r="F51">
+        <v>0.5</v>
+      </c>
+      <c r="G51">
+        <v>7.5</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>134</v>
+      </c>
+      <c r="G52">
+        <v>7.5</v>
+      </c>
+      <c r="H52">
+        <f>F52+G52</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E53" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="D53" t="s">
+        <v>144</v>
+      </c>
+      <c r="G53">
+        <v>7.5</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>120</v>
+        <v>149</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
-      </c>
-      <c r="G54" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="G54">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4530,8 +4736,12 @@
       <c r="E55" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <f>F55+G55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4544,100 +4754,104 @@
       <c r="D56" t="s">
         <v>135</v>
       </c>
-      <c r="G56" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>7.5</v>
+      </c>
+      <c r="H56">
+        <f>F56+G56</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
-        <v>155</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="M59" s="5">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>157</v>
-      </c>
-      <c r="M60" s="5">
-        <v>42695</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="M60" t="s">
+        <v>132</v>
+      </c>
+      <c r="N60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>159</v>
-      </c>
-      <c r="M61" t="s">
-        <v>132</v>
-      </c>
-      <c r="N61" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>164</v>
+      </c>
       <c r="D62" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>168</v>
-      </c>
-      <c r="D63" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>169</v>
-      </c>
-      <c r="D64" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>171</v>
       </c>
       <c r="D66" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>172</v>
       </c>
-      <c r="D67" t="s">
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4657,7 +4871,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>